<commit_message>
ashley = 1, code = 0
</commit_message>
<xml_diff>
--- a/spreadsheets/Archives/OldForms/last8pForm.xlsx
+++ b/spreadsheets/Archives/OldForms/last8pForm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18975" windowHeight="5070" xr2:uid="{3E72FD45-E12F-46E9-A8CF-A344301911B1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18975" windowHeight="5070" xr2:uid="{C77065BD-5F8F-4625-A791-E7B561F338E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Date Stamp</t>
   </si>
@@ -39,15 +39,63 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NOT A COMMENT</t>
+  </si>
+  <si>
+    <t>KH</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>90A,92B</t>
+  </si>
+  <si>
+    <t>KC</t>
+  </si>
+  <si>
+    <t>883,92A</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>91A,98B</t>
+  </si>
+  <si>
+    <t>DG</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>LG</t>
+  </si>
+  <si>
+    <t>KGH</t>
+  </si>
+  <si>
+    <t>JW</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -118,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -126,9 +174,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -139,7 +184,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -149,9 +194,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -166,9 +208,6 @@
     </xf>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -207,7 +246,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5080C1D-58F3-4757-A097-4CB230248571}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B86AE6C7-C29D-4CA9-95D0-0A8EC629D552}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -541,7 +580,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE244E37-6386-435B-9BE4-140C70A72979}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80E647F-1A16-4D37-BF12-5475F9F5CF05}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F28"/>
   <sheetViews>
@@ -551,14 +590,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="18" customWidth="1"/>
-    <col min="5" max="5" width="42.7109375" style="16" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" style="15" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="16.5703125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="14" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -571,227 +610,313 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="6"/>
+      <c r="A2" s="4">
+        <v>43067</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="7">
+        <v>880881</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="6"/>
+      <c r="A3" s="4">
+        <v>43067</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="6"/>
+      <c r="A4" s="4">
+        <v>43067</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="6"/>
+      <c r="A5" s="4">
+        <v>43067</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="6"/>
+      <c r="A6" s="4">
+        <v>43067</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7">
+        <v>882886</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="6"/>
+      <c r="A7" s="4">
+        <v>43067</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7">
+        <v>880881</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="6"/>
+      <c r="A8" s="4">
+        <v>43067</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="6"/>
+      <c r="A9" s="4">
+        <v>43067</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="6"/>
+      <c r="A10" s="4">
+        <v>43067</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="6"/>
+      <c r="A11" s="4">
+        <v>43067</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="7">
+        <v>882886</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="6"/>
+      <c r="A12" s="4">
+        <v>43068</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="6"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="6"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="6"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="6"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="6"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="6"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="6"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="6"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="6"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="6"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="6"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="6"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="6"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="6"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="6"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="6"/>
+      <c r="A28" s="4"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>